<commit_message>
Add documentation, presentation and test plan
</commit_message>
<xml_diff>
--- a/documents/QA - UnitTesting - Ace of Spades.xlsx
+++ b/documents/QA - UnitTesting - Ace of Spades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teodor Madjarov\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PGKPI\Ace-of-Spades\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8761ADFB-FF00-4D6D-A3C2-B77ACE3D02CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F24BCA4-EE4F-426E-B120-A415882BC61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B952D1FD-FFD1-437D-96A0-DCBAAD4D345D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B952D1FD-FFD1-437D-96A0-DCBAAD4D345D}"/>
   </bookViews>
   <sheets>
     <sheet name="Unit testing" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,79 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -443,101 +515,29 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,66 +893,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1"/>
@@ -970,36 +970,36 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1"/>
@@ -1017,97 +1017,97 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" ht="21">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="16" t="s">
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17" t="s">
+      <c r="H10" s="37"/>
+      <c r="I10" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="43">
         <v>44909</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17" t="s">
+      <c r="H12" s="37"/>
+      <c r="I12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1"/>
@@ -1125,140 +1125,140 @@
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" ht="18.75">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="16" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16" t="s">
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16" t="s">
+      <c r="H15" s="37"/>
+      <c r="I15" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="16"/>
+      <c r="J15" s="37"/>
       <c r="K15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="16"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="1:13" ht="18.75">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="41" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="41">
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15">
         <v>1</v>
       </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="33" t="s">
+      <c r="H16" s="16"/>
+      <c r="I16" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="34"/>
+      <c r="J16" s="31"/>
       <c r="K16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="L16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="34"/>
+      <c r="M16" s="31"/>
     </row>
     <row r="17" spans="1:13" ht="18.75">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="44">
+      <c r="B17" s="14"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="19">
         <v>2</v>
       </c>
-      <c r="H17" s="46"/>
-      <c r="I17" s="44" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="46"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="37" t="s">
+      <c r="L17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M17" s="38"/>
+      <c r="M17" s="29"/>
     </row>
     <row r="18" spans="1:13" ht="18.75">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="39">
+      <c r="B18" s="25"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="17">
         <v>3</v>
       </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="39" t="s">
+      <c r="H18" s="22"/>
+      <c r="I18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="40"/>
+      <c r="J18" s="22"/>
       <c r="K18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="35" t="s">
+      <c r="L18" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M18" s="36"/>
+      <c r="M18" s="27"/>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1"/>
@@ -1276,97 +1276,97 @@
       <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:13" ht="21">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="37"/>
+      <c r="C25" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="16" t="s">
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17" t="s">
+      <c r="H25" s="37"/>
+      <c r="I25" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="25">
+      <c r="B27" s="14"/>
+      <c r="C27" s="43">
         <v>44909</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="16" t="s">
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="17" t="s">
+      <c r="H27" s="37"/>
+      <c r="I27" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1"/>
@@ -1384,190 +1384,190 @@
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="27" t="s">
+      <c r="B30" s="45"/>
+      <c r="C30" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27" t="s">
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27" t="s">
+      <c r="H30" s="46"/>
+      <c r="I30" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="J30" s="27"/>
+      <c r="J30" s="46"/>
       <c r="K30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="27" t="s">
+      <c r="L30" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="27"/>
+      <c r="M30" s="46"/>
     </row>
     <row r="31" spans="1:13" ht="18.75">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="41" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="41">
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="15">
         <v>1</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="41" t="s">
+      <c r="H31" s="21"/>
+      <c r="I31" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J31" s="43"/>
+      <c r="J31" s="16"/>
       <c r="K31" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L31" s="33" t="s">
+      <c r="L31" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M31" s="34"/>
+      <c r="M31" s="31"/>
     </row>
     <row r="32" spans="1:13" ht="18.75">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="44">
+      <c r="B32" s="14"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="19">
         <v>2</v>
       </c>
-      <c r="H32" s="45"/>
-      <c r="I32" s="44" t="s">
+      <c r="H32" s="20"/>
+      <c r="I32" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="46"/>
+      <c r="J32" s="23"/>
       <c r="K32" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L32" s="37" t="s">
+      <c r="L32" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M32" s="38"/>
+      <c r="M32" s="29"/>
     </row>
     <row r="33" spans="1:13" ht="18.75">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="44">
+      <c r="B33" s="14"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="19">
         <v>3</v>
       </c>
-      <c r="H33" s="45"/>
-      <c r="I33" s="44" t="s">
+      <c r="H33" s="20"/>
+      <c r="I33" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J33" s="46"/>
+      <c r="J33" s="23"/>
       <c r="K33" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L33" s="37" t="s">
+      <c r="L33" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="38"/>
+      <c r="M33" s="29"/>
     </row>
     <row r="34" spans="1:13" ht="18.75">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="44">
+      <c r="B34" s="14"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="19">
         <v>4</v>
       </c>
-      <c r="H34" s="45"/>
-      <c r="I34" s="44" t="s">
+      <c r="H34" s="20"/>
+      <c r="I34" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="J34" s="46"/>
+      <c r="J34" s="23"/>
       <c r="K34" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L34" s="37" t="s">
+      <c r="L34" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="M34" s="38"/>
+      <c r="M34" s="29"/>
     </row>
     <row r="35" spans="1:13" ht="18.75">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="39">
+      <c r="B35" s="25"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="17">
         <v>5</v>
       </c>
-      <c r="H35" s="47"/>
-      <c r="I35" s="39" t="s">
+      <c r="H35" s="18"/>
+      <c r="I35" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="J35" s="40"/>
+      <c r="J35" s="22"/>
       <c r="K35" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L35" s="35" t="s">
+      <c r="L35" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="M35" s="36"/>
+      <c r="M35" s="27"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="38"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
+      <c r="A39" s="38"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1"/>
@@ -1585,97 +1585,97 @@
       <c r="M40" s="3"/>
     </row>
     <row r="41" spans="1:13" ht="21">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="39"/>
+      <c r="M41" s="39"/>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17" t="s">
+      <c r="B42" s="37"/>
+      <c r="C42" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="16" t="s">
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H42" s="16"/>
-      <c r="I42" s="17" t="s">
+      <c r="H42" s="37"/>
+      <c r="I42" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="36"/>
+      <c r="M42" s="36"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="17"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="17"/>
-      <c r="L43" s="17"/>
-      <c r="M43" s="17"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="25">
+      <c r="B44" s="14"/>
+      <c r="C44" s="43">
         <v>44909</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="16" t="s">
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H44" s="16"/>
-      <c r="I44" s="17" t="s">
+      <c r="H44" s="37"/>
+      <c r="I44" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="J44" s="17"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="23"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="17"/>
-      <c r="L45" s="17"/>
-      <c r="M45" s="17"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="1"/>
@@ -1693,87 +1693,104 @@
       <c r="M46" s="3"/>
     </row>
     <row r="47" spans="1:13" ht="18.75">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="16" t="s">
+      <c r="B47" s="44"/>
+      <c r="C47" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16" t="s">
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16" t="s">
+      <c r="H47" s="37"/>
+      <c r="I47" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J47" s="16"/>
+      <c r="J47" s="37"/>
       <c r="K47" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L47" s="16" t="s">
+      <c r="L47" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="M47" s="16"/>
+      <c r="M47" s="37"/>
     </row>
     <row r="48" spans="1:13" ht="37.5">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="30" t="s">
+      <c r="B48" s="25"/>
+      <c r="C48" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="28" t="s">
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="H48" s="29"/>
-      <c r="I48" s="28" t="s">
+      <c r="H48" s="35"/>
+      <c r="I48" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="J48" s="29"/>
+      <c r="J48" s="35"/>
       <c r="K48" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L48" s="30" t="s">
+      <c r="L48" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="M48" s="32"/>
+      <c r="M48" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C16:F18"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A1:M4"/>
+    <mergeCell ref="A6:M7"/>
+    <mergeCell ref="A9:M9"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:F11"/>
+    <mergeCell ref="G10:H11"/>
+    <mergeCell ref="I10:M11"/>
+    <mergeCell ref="G12:H13"/>
+    <mergeCell ref="I12:M13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="C12:F13"/>
+    <mergeCell ref="A21:M22"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:B26"/>
+    <mergeCell ref="C25:F26"/>
+    <mergeCell ref="G25:H26"/>
+    <mergeCell ref="I25:M26"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="C27:F28"/>
+    <mergeCell ref="G27:H28"/>
+    <mergeCell ref="I27:M28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="C44:F45"/>
+    <mergeCell ref="G44:H45"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:F47"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="L17:M17"/>
@@ -1790,49 +1807,32 @@
     <mergeCell ref="G42:H43"/>
     <mergeCell ref="I42:M43"/>
     <mergeCell ref="C31:F35"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="C44:F45"/>
-    <mergeCell ref="G44:H45"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:F47"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:F28"/>
-    <mergeCell ref="G27:H28"/>
-    <mergeCell ref="I27:M28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="A21:M22"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A25:B26"/>
-    <mergeCell ref="C25:F26"/>
-    <mergeCell ref="G25:H26"/>
-    <mergeCell ref="I25:M26"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="C12:F13"/>
-    <mergeCell ref="G12:H13"/>
-    <mergeCell ref="I12:M13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="A1:M4"/>
-    <mergeCell ref="A6:M7"/>
-    <mergeCell ref="A9:M9"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C10:F11"/>
-    <mergeCell ref="G10:H11"/>
-    <mergeCell ref="I10:M11"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="C16:F18"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A32:B32"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="I12:M13 I27:M28 I44:M45 L16:L18 L31:L35 L48">

</xml_diff>